<commit_message>
Added version of Education averages file which is easier to import
</commit_message>
<xml_diff>
--- a/data/data-education-modified/education-averages.xlsx
+++ b/data/data-education-modified/education-averages.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fergu\Documents\Work\Ironhack\Projects\Mini-project-2\Mini-project-London\Education Data\Modified Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fergu\Documents\Work\Ironhack\Projects\Mini-project-2\Mini-project-London\data\data-education-modified\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -130,15 +130,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="104">
   <si>
     <t>Average Attainment 8 score per pupil</t>
   </si>
   <si>
     <t>Average Progress 8 score per pupil</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>Code</t>
@@ -1029,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,44 +1043,44 @@
       <c r="A1" s="2"/>
       <c r="B1" s="24"/>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="35"/>
       <c r="I1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="G2" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>103</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>104</v>
       </c>
       <c r="I2" s="22" t="s">
         <v>0</v>
@@ -1106,10 +1103,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="8"/>
@@ -1117,19 +1114,15 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="27"/>
-      <c r="I4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="14">
         <v>75.375</v>
@@ -1158,10 +1151,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>10</v>
       </c>
       <c r="C6" s="14">
         <v>77.8125</v>
@@ -1190,10 +1183,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="14">
         <v>80.375</v>
@@ -1222,10 +1215,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>14</v>
       </c>
       <c r="C8" s="14">
         <v>74.375</v>
@@ -1254,10 +1247,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>16</v>
       </c>
       <c r="C9" s="14">
         <v>80.3125</v>
@@ -1286,10 +1279,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>18</v>
       </c>
       <c r="C10" s="14">
         <v>75.4375</v>
@@ -1318,10 +1311,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>20</v>
       </c>
       <c r="C11" s="14">
         <v>77</v>
@@ -1350,10 +1343,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>22</v>
       </c>
       <c r="C12" s="14">
         <v>74.5</v>
@@ -1382,10 +1375,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>24</v>
       </c>
       <c r="C13" s="14">
         <v>72.1875</v>
@@ -1414,10 +1407,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>26</v>
       </c>
       <c r="C14" s="14">
         <v>80.3125</v>
@@ -1446,10 +1439,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>28</v>
       </c>
       <c r="C15" s="14">
         <v>80.75</v>
@@ -1478,10 +1471,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>30</v>
       </c>
       <c r="C16" s="14">
         <v>78.75</v>
@@ -1510,10 +1503,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="34" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>32</v>
       </c>
       <c r="C17" s="14">
         <v>78.125</v>
@@ -1542,10 +1535,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="34" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>34</v>
       </c>
       <c r="C18" s="14">
         <v>78.875</v>
@@ -1574,10 +1567,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="34" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>36</v>
       </c>
       <c r="C19" s="14">
         <v>78.125</v>
@@ -1606,10 +1599,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>38</v>
       </c>
       <c r="C20" s="14">
         <v>76.0625</v>
@@ -1638,10 +1631,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="34" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>40</v>
       </c>
       <c r="C21" s="14">
         <v>79.875</v>
@@ -1670,10 +1663,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>42</v>
       </c>
       <c r="C22" s="14">
         <v>75.8125</v>
@@ -1702,10 +1695,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="34" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>44</v>
       </c>
       <c r="C23" s="14">
         <v>81.0625</v>
@@ -1734,10 +1727,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>45</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>46</v>
       </c>
       <c r="C24" s="14">
         <v>78.6875</v>
@@ -1766,10 +1759,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="34" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>48</v>
       </c>
       <c r="C25" s="14">
         <v>78.8125</v>
@@ -1798,10 +1791,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="34" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>50</v>
       </c>
       <c r="C26" s="14">
         <v>78.0625</v>
@@ -1830,10 +1823,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="34" t="s">
         <v>51</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>52</v>
       </c>
       <c r="C27" s="14">
         <v>77.125</v>
@@ -1862,10 +1855,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="34" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>54</v>
       </c>
       <c r="C28" s="14">
         <v>79.0625</v>
@@ -1894,10 +1887,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>56</v>
       </c>
       <c r="C29" s="14">
         <v>78.1875</v>
@@ -1926,10 +1919,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="34" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>58</v>
       </c>
       <c r="C30" s="14">
         <v>82</v>
@@ -1958,10 +1951,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="34" t="s">
         <v>59</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>60</v>
       </c>
       <c r="C31" s="14">
         <v>77.75</v>
@@ -1990,10 +1983,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="34" t="s">
         <v>61</v>
-      </c>
-      <c r="B32" s="34" t="s">
-        <v>62</v>
       </c>
       <c r="C32" s="14">
         <v>78.8125</v>
@@ -2022,10 +2015,10 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="34" t="s">
         <v>63</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>64</v>
       </c>
       <c r="C33" s="14">
         <v>76.25</v>
@@ -2054,10 +2047,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="34" t="s">
         <v>65</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>66</v>
       </c>
       <c r="C34" s="14">
         <v>79.9375</v>
@@ -2086,10 +2079,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="34" t="s">
         <v>67</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>68</v>
       </c>
       <c r="C35" s="14">
         <v>81.0625</v>
@@ -2118,10 +2111,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="34" t="s">
         <v>69</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>70</v>
       </c>
       <c r="C36" s="14">
         <v>76.6875</v>
@@ -2152,17 +2145,17 @@
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H37" s="29"/>
       <c r="I37" s="11"/>
@@ -2170,10 +2163,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="34" t="s">
         <v>71</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>72</v>
       </c>
       <c r="C38" s="14">
         <v>78.4375</v>
@@ -2202,10 +2195,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="34" t="s">
         <v>73</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>74</v>
       </c>
       <c r="C39" s="14">
         <v>77.625</v>
@@ -2236,17 +2229,17 @@
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
       <c r="C40" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H40" s="29"/>
       <c r="I40" s="11"/>
@@ -2254,10 +2247,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="34" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>76</v>
       </c>
       <c r="C41" s="14">
         <v>76.4375</v>
@@ -2286,10 +2279,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="34" t="s">
         <v>77</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>78</v>
       </c>
       <c r="C42" s="14">
         <v>73.25</v>
@@ -2318,10 +2311,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="34" t="s">
         <v>79</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>80</v>
       </c>
       <c r="C43" s="14">
         <v>72.5625</v>
@@ -2350,10 +2343,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="34" t="s">
         <v>81</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>82</v>
       </c>
       <c r="C44" s="14">
         <v>73.4375</v>
@@ -2382,10 +2375,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="34" t="s">
         <v>83</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>84</v>
       </c>
       <c r="C45" s="14">
         <v>73.75</v>
@@ -2414,10 +2407,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="34" t="s">
         <v>85</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>86</v>
       </c>
       <c r="C46" s="14">
         <v>75.25</v>
@@ -2446,10 +2439,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>88</v>
       </c>
       <c r="C47" s="14">
         <v>77.75</v>
@@ -2478,10 +2471,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>90</v>
       </c>
       <c r="C48" s="14">
         <v>77.0625</v>
@@ -2510,10 +2503,10 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="34" t="s">
         <v>91</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>92</v>
       </c>
       <c r="C49" s="14">
         <v>75.0625</v>
@@ -2544,17 +2537,17 @@
       <c r="A50" s="13"/>
       <c r="B50" s="16"/>
       <c r="C50" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H50" s="29"/>
       <c r="I50" s="1"/>
@@ -2562,10 +2555,10 @@
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="32" t="s">
         <v>93</v>
-      </c>
-      <c r="B51" s="32" t="s">
-        <v>94</v>
       </c>
       <c r="C51" s="17">
         <v>75.125</v>

</xml_diff>